<commit_message>
Added Upload Profile Test with Excel connect
</commit_message>
<xml_diff>
--- a/test_data/orange_test_data.xlsx
+++ b/test_data/orange_test_data.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test_add_valid_employee" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="test_invalid_profile_upload" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>User Name</t>
   </si>
@@ -68,6 +68,24 @@
   </si>
   <si>
     <t>Ken kevin</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Upload File Detail</t>
+  </si>
+  <si>
+    <t>Expected Error</t>
+  </si>
+  <si>
+    <t>C:\Mine\Balaji-Profile_2023.pdf</t>
+  </si>
+  <si>
+    <t>C:\Mine\iFuture.txt</t>
+  </si>
+  <si>
+    <t>File type not allowed</t>
   </si>
 </sst>
 </file>
@@ -387,7 +405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -455,13 +473,64 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>